<commit_message>
adjust function bepaal_N_vak to rode draad nr. 10
</commit_message>
<xml_diff>
--- a/workspace/output/Vakkansen_voorbeeld.xlsx
+++ b/workspace/output/Vakkansen_voorbeeld.xlsx
@@ -559,10 +559,10 @@
         </is>
       </c>
       <c r="N2" t="n">
-        <v>2.755</v>
+        <v>1.755</v>
       </c>
       <c r="O2" t="n">
-        <v>0.002451067615658363</v>
+        <v>0.001561387900355872</v>
       </c>
     </row>
     <row r="3">
@@ -614,10 +614,10 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>3.37342</v>
+        <v>2.37342</v>
       </c>
       <c r="O3" t="n">
-        <v>0.00313806511627907</v>
+        <v>0.002207832558139535</v>
       </c>
     </row>
     <row r="4">
@@ -669,10 +669,10 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>2.06008</v>
+        <v>1.06008</v>
       </c>
       <c r="O4" t="n">
-        <v>0.001013320216428923</v>
+        <v>0.0005214363010329562</v>
       </c>
     </row>
     <row r="5">
@@ -724,10 +724,10 @@
         </is>
       </c>
       <c r="N5" t="n">
-        <v>3.2995</v>
+        <v>2.2995</v>
       </c>
       <c r="O5" t="n">
-        <v>0.003052266419981499</v>
+        <v>0.002127197039777983</v>
       </c>
     </row>
     <row r="6">
@@ -779,10 +779,10 @@
         </is>
       </c>
       <c r="N6" t="n">
-        <v>1.438</v>
+        <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>7.161354581673307e-05</v>
+        <v>4.980079681274901e-05</v>
       </c>
     </row>
     <row r="7">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="N7" t="n">
-        <v>1.495</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>1.312610004620387e-08</v>
+        <v>8.7800000309056e-09</v>
       </c>
     </row>
     <row r="8">
@@ -889,10 +889,10 @@
         </is>
       </c>
       <c r="N8" t="n">
-        <v>2.18968</v>
+        <v>1.18968</v>
       </c>
       <c r="O8" t="n">
-        <v>1.449568177394818e-06</v>
+        <v>7.87568169450818e-07</v>
       </c>
     </row>
     <row r="9">
@@ -944,10 +944,10 @@
         </is>
       </c>
       <c r="N9" t="n">
-        <v>1.86067</v>
+        <v>1</v>
       </c>
       <c r="O9" t="n">
-        <v>1.432717332717333e-05</v>
+        <v>7.700007700007701e-06</v>
       </c>
     </row>
     <row r="10">
@@ -999,10 +999,10 @@
         </is>
       </c>
       <c r="N10" t="n">
-        <v>5.100580000000003</v>
+        <v>4.100580000000003</v>
       </c>
       <c r="O10" t="n">
-        <v>3.493906908244e-05</v>
+        <v>2.808905024488819e-05</v>
       </c>
     </row>
     <row r="11">
@@ -1054,10 +1054,10 @@
         </is>
       </c>
       <c r="N11" t="n">
-        <v>3.652029999999998</v>
+        <v>2.652029999999998</v>
       </c>
       <c r="O11" t="n">
-        <v>7.632741097124365e-06</v>
+        <v>5.542741536024272e-06</v>
       </c>
     </row>
     <row r="12">
@@ -1109,10 +1109,10 @@
         </is>
       </c>
       <c r="N12" t="n">
-        <v>3.03712</v>
+        <v>2.03712</v>
       </c>
       <c r="O12" t="n">
-        <v>0.00109643321299639</v>
+        <v>0.00073542238267148</v>
       </c>
     </row>
     <row r="13">
@@ -1164,10 +1164,10 @@
         </is>
       </c>
       <c r="N13" t="n">
-        <v>3.614920000000001</v>
+        <v>2.614920000000001</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0002460468282058264</v>
+        <v>0.0001779825755513205</v>
       </c>
     </row>
     <row r="14">
@@ -1219,10 +1219,10 @@
         </is>
       </c>
       <c r="N14" t="n">
-        <v>1.982560000000001</v>
+        <v>1</v>
       </c>
       <c r="O14" t="n">
-        <v>8.584368911019707e-05</v>
+        <v>4.329941545789132e-05</v>
       </c>
     </row>
     <row r="15">
@@ -1274,10 +1274,10 @@
         </is>
       </c>
       <c r="N15" t="n">
-        <v>1.53073</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
-        <v>1.790954099999999e-88</v>
+        <v>1.17e-88</v>
       </c>
     </row>
     <row r="16">
@@ -1329,10 +1329,10 @@
         </is>
       </c>
       <c r="N16" t="n">
-        <v>2.91649</v>
+        <v>1.91649</v>
       </c>
       <c r="O16" t="n">
-        <v>0.00291066866267465</v>
+        <v>0.001912664670658683</v>
       </c>
     </row>
     <row r="17">
@@ -1384,10 +1384,10 @@
         </is>
       </c>
       <c r="N17" t="n">
-        <v>1.942119999999997</v>
+        <v>1</v>
       </c>
       <c r="O17" t="n">
-        <v>2.31111216888402e-05</v>
+        <v>1.18999452602518e-05</v>
       </c>
     </row>
     <row r="18">
@@ -1439,10 +1439,10 @@
         </is>
       </c>
       <c r="N18" t="n">
-        <v>1.89451</v>
+        <v>1</v>
       </c>
       <c r="O18" t="n">
-        <v>1.328051066430944e-06</v>
+        <v>7.009997658660782e-07</v>
       </c>
     </row>
     <row r="19">
@@ -1494,10 +1494,10 @@
         </is>
       </c>
       <c r="N19" t="n">
-        <v>1.319650000000003</v>
+        <v>1</v>
       </c>
       <c r="O19" t="n">
-        <v>1.080794430794434e-05</v>
+        <v>8.190008190008191e-06</v>
       </c>
     </row>
     <row r="20">
@@ -1549,10 +1549,10 @@
         </is>
       </c>
       <c r="N20" t="n">
-        <v>1.877290000000001</v>
+        <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>6.157512185201953e-07</v>
+        <v>3.280000524800084e-07</v>
       </c>
     </row>
     <row r="21">
@@ -1604,10 +1604,10 @@
         </is>
       </c>
       <c r="N21" t="n">
-        <v>2.160010000000001</v>
+        <v>1.16001</v>
       </c>
       <c r="O21" t="n">
-        <v>2.678411114362666e-06</v>
+        <v>1.43841170956238e-06</v>
       </c>
     </row>
     <row r="22">
@@ -1659,10 +1659,10 @@
         </is>
       </c>
       <c r="N22" t="n">
-        <v>1.243869999999997</v>
+        <v>1</v>
       </c>
       <c r="O22" t="n">
-        <v>2.41310780012065e-10</v>
+        <v>1.940000000097e-10</v>
       </c>
     </row>
     <row r="23">
@@ -1714,10 +1714,10 @@
         </is>
       </c>
       <c r="N23" t="n">
-        <v>3.688060000000001</v>
+        <v>2.688060000000001</v>
       </c>
       <c r="O23" t="n">
-        <v>1.759204620000176e-11</v>
+        <v>1.282204620000129e-11</v>
       </c>
     </row>
     <row r="24">
@@ -1769,10 +1769,10 @@
         </is>
       </c>
       <c r="N24" t="n">
-        <v>1.402</v>
+        <v>1</v>
       </c>
       <c r="O24" t="n">
-        <v>7.725028652032091e-06</v>
+        <v>5.510006171206912e-06</v>
       </c>
     </row>
     <row r="25">
@@ -1824,10 +1824,10 @@
         </is>
       </c>
       <c r="N25" t="n">
-        <v>1.449129999999997</v>
+        <v>1</v>
       </c>
       <c r="O25" t="n">
-        <v>1.334648766969768e-07</v>
+        <v>9.210000255117007e-08</v>
       </c>
     </row>
     <row r="26">
@@ -1879,10 +1879,10 @@
         </is>
       </c>
       <c r="N26" t="n">
-        <v>1.821580000000002</v>
+        <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>7.122502443792774e-05</v>
+        <v>3.910068426197458e-05</v>
       </c>
     </row>
     <row r="27">
@@ -1934,10 +1934,10 @@
         </is>
       </c>
       <c r="N27" t="n">
-        <v>1.741</v>
+        <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>4.735482116143071e-05</v>
+        <v>2.719978240174079e-05</v>
       </c>
     </row>
     <row r="28">
@@ -1989,10 +1989,10 @@
         </is>
       </c>
       <c r="N28" t="n">
-        <v>1.508379999999997</v>
+        <v>1</v>
       </c>
       <c r="O28" t="n">
-        <v>4.872028423772601e-05</v>
+        <v>3.229974160206718e-05</v>
       </c>
     </row>
     <row r="29">
@@ -2044,10 +2044,10 @@
         </is>
       </c>
       <c r="N29" t="n">
-        <v>1.60402</v>
+        <v>1</v>
       </c>
       <c r="O29" t="n">
-        <v>0.0001892648967551623</v>
+        <v>0.0001179941002949853</v>
       </c>
     </row>
     <row r="30">
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="N30" t="n">
-        <v>2.551540000000001</v>
+        <v>1.551540000000001</v>
       </c>
       <c r="O30" t="n">
-        <v>1.178812658812659e-05</v>
+        <v>7.168121968121971e-06</v>
       </c>
     </row>
     <row r="31">
@@ -2154,10 +2154,10 @@
         </is>
       </c>
       <c r="N31" t="n">
-        <v>2.96851</v>
+        <v>1.96851</v>
       </c>
       <c r="O31" t="n">
-        <v>9.825761713254888e-06</v>
+        <v>6.51576386475349e-06</v>
       </c>
     </row>
     <row r="32">
@@ -2209,10 +2209,10 @@
         </is>
       </c>
       <c r="N32" t="n">
-        <v>3.108550000000001</v>
+        <v>2.108550000000001</v>
       </c>
       <c r="O32" t="n">
-        <v>2.048535371840918e-05</v>
+        <v>1.389535075290785e-05</v>
       </c>
     </row>
     <row r="33">
@@ -2264,10 +2264,10 @@
         </is>
       </c>
       <c r="N33" t="n">
-        <v>3.424</v>
+        <v>2.424</v>
       </c>
       <c r="O33" t="n">
-        <v>3.112727272727273e-07</v>
+        <v>2.203636363636364e-07</v>
       </c>
     </row>
     <row r="34">
@@ -2319,10 +2319,10 @@
         </is>
       </c>
       <c r="N34" t="n">
-        <v>4.554969999999999</v>
+        <v>3.554969999999999</v>
       </c>
       <c r="O34" t="n">
-        <v>0.000701412072682476</v>
+        <v>0.0005474237757930396</v>
       </c>
     </row>
     <row r="35">
@@ -2374,10 +2374,10 @@
         </is>
       </c>
       <c r="N35" t="n">
-        <v>1.969780000000001</v>
+        <v>1</v>
       </c>
       <c r="O35" t="n">
-        <v>1.215353917270196e-06</v>
+        <v>6.169998260060491e-07</v>
       </c>
     </row>
     <row r="36">
@@ -2429,10 +2429,10 @@
         </is>
       </c>
       <c r="N36" t="n">
-        <v>1.914279999999995</v>
+        <v>1</v>
       </c>
       <c r="O36" t="n">
-        <v>3.369131721877841e-06</v>
+        <v>1.75999943680018e-06</v>
       </c>
     </row>
     <row r="37">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="N37" t="n">
-        <v>2.723620000000003</v>
+        <v>1.723620000000003</v>
       </c>
       <c r="O37" t="n">
-        <v>6.209853617387596e-08</v>
+        <v>3.929853611003596e-08</v>
       </c>
     </row>
     <row r="38">
@@ -2539,10 +2539,10 @@
         </is>
       </c>
       <c r="N38" t="n">
-        <v>1.860820000000007</v>
+        <v>1</v>
       </c>
       <c r="O38" t="n">
-        <v>4.875340599455059e-05</v>
+        <v>2.619995808006707e-05</v>
       </c>
     </row>
     <row r="39">
@@ -2594,10 +2594,10 @@
         </is>
       </c>
       <c r="N39" t="n">
-        <v>1.179069999999996</v>
+        <v>1</v>
       </c>
       <c r="O39" t="n">
-        <v>1.006925941108147e-05</v>
+        <v>8.540001366400219e-06</v>
       </c>
     </row>
     <row r="40">
@@ -2649,10 +2649,10 @@
         </is>
       </c>
       <c r="N40" t="n">
-        <v>4.154830000000002</v>
+        <v>3.154830000000002</v>
       </c>
       <c r="O40" t="n">
-        <v>4.944248491079762e-06</v>
+        <v>3.75424830067973e-06</v>
       </c>
     </row>
     <row r="41">
@@ -2704,10 +2704,10 @@
         </is>
       </c>
       <c r="N41" t="n">
-        <v>2.432949999999994</v>
+        <v>1.432949999999994</v>
       </c>
       <c r="O41" t="n">
-        <v>6.349995563002735e-06</v>
+        <v>3.739997181201731e-06</v>
       </c>
     </row>
     <row r="42">
@@ -2759,10 +2759,10 @@
         </is>
       </c>
       <c r="N42" t="n">
-        <v>2.090200000000004</v>
+        <v>1.090200000000004</v>
       </c>
       <c r="O42" t="n">
-        <v>6.939575033200545e-05</v>
+        <v>3.619521912350612e-05</v>
       </c>
     </row>
     <row r="43">
@@ -2814,10 +2814,10 @@
         </is>
       </c>
       <c r="N43" t="n">
-        <v>1.648390000000003</v>
+        <v>1</v>
       </c>
       <c r="O43" t="n">
-        <v>3.098973197768746e-09</v>
+        <v>1.8799999986464e-09</v>
       </c>
     </row>
     <row r="44">
@@ -2869,10 +2869,10 @@
         </is>
       </c>
       <c r="N44" t="n">
-        <v>2.62723</v>
+        <v>1.62723</v>
       </c>
       <c r="O44" t="n">
-        <v>2.149074118079444e-07</v>
+        <v>1.331074126423044e-07</v>
       </c>
     </row>
     <row r="45">
@@ -2924,10 +2924,10 @@
         </is>
       </c>
       <c r="N45" t="n">
-        <v>2.008929999999993</v>
+        <v>1.008929999999993</v>
       </c>
       <c r="O45" t="n">
-        <v>4.178574667428765e-07</v>
+        <v>2.098574534308756e-07</v>
       </c>
     </row>
     <row r="46">
@@ -2979,10 +2979,10 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>1.983700000000004</v>
+        <v>1</v>
       </c>
       <c r="O46" t="n">
-        <v>4.760876191299057e-06</v>
+        <v>2.399998080001536e-06</v>
       </c>
     </row>
     <row r="47">
@@ -3034,10 +3034,10 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>1.758729999999999</v>
+        <v>1</v>
       </c>
       <c r="O47" t="n">
-        <v>1.681345887397921e-07</v>
+        <v>9.560000042064e-08</v>
       </c>
     </row>
     <row r="48">
@@ -3089,10 +3089,10 @@
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3.478779999999995</v>
+        <v>2.478779999999995</v>
       </c>
       <c r="O48" t="n">
-        <v>3.064805125446465e-07</v>
+        <v>2.183805141128264e-07</v>
       </c>
     </row>
     <row r="49">
@@ -3144,10 +3144,10 @@
         </is>
       </c>
       <c r="N49" t="n">
-        <v>2.587720000000005</v>
+        <v>1.587720000000005</v>
       </c>
       <c r="O49" t="n">
-        <v>2.385877836659776e-07</v>
+        <v>1.463877837950576e-07</v>
       </c>
     </row>
     <row r="50">
@@ -3199,10 +3199,10 @@
         </is>
       </c>
       <c r="N50" t="n">
-        <v>4.405810000000001</v>
+        <v>3.405810000000001</v>
       </c>
       <c r="O50" t="n">
-        <v>3.225052963860721e-07</v>
+        <v>2.493052953905521e-07</v>
       </c>
     </row>
     <row r="51">
@@ -3254,10 +3254,10 @@
         </is>
       </c>
       <c r="N51" t="n">
-        <v>5.234949999999993</v>
+        <v>4.234949999999993</v>
       </c>
       <c r="O51" t="n">
-        <v>2.041632541632539e-05</v>
+        <v>1.651632151632149e-05</v>
       </c>
     </row>
     <row r="52">
@@ -3309,10 +3309,10 @@
         </is>
       </c>
       <c r="N52" t="n">
-        <v>2.068240000000005</v>
+        <v>1.068240000000005</v>
       </c>
       <c r="O52" t="n">
-        <v>1.629773123846269e-08</v>
+        <v>8.417731219865887e-09</v>
       </c>
     </row>
     <row r="53">
@@ -3364,10 +3364,10 @@
         </is>
       </c>
       <c r="N53" t="n">
-        <v>1.625560000000001</v>
+        <v>1</v>
       </c>
       <c r="O53" t="n">
-        <v>3.251120000000003e-09</v>
+        <v>2e-09</v>
       </c>
     </row>
     <row r="54">
@@ -3419,10 +3419,10 @@
         </is>
       </c>
       <c r="N54" t="n">
-        <v>1.916649999999998</v>
+        <v>1</v>
       </c>
       <c r="O54" t="n">
-        <v>1.721151693975967e-08</v>
+        <v>8.97999996857e-09</v>
       </c>
     </row>
     <row r="55">
@@ -3474,10 +3474,10 @@
         </is>
       </c>
       <c r="N55" t="n">
-        <v>2.004970000000005</v>
+        <v>1.004970000000005</v>
       </c>
       <c r="O55" t="n">
-        <v>3.388399301897512e-09</v>
+        <v>1.698399300951112e-09</v>
       </c>
     </row>
     <row r="56">
@@ -3529,10 +3529,10 @@
         </is>
       </c>
       <c r="N56" t="n">
-        <v>4.892949999999994</v>
+        <v>3.892949999999994</v>
       </c>
       <c r="O56" t="n">
-        <v>2.994485396526393e-08</v>
+        <v>2.382485397236313e-08</v>
       </c>
     </row>
     <row r="57">
@@ -3584,10 +3584,10 @@
         </is>
       </c>
       <c r="N57" t="n">
-        <v>2.544580000000002</v>
+        <v>1.544580000000002</v>
       </c>
       <c r="O57" t="n">
-        <v>9.313162799858445e-11</v>
+        <v>5.653162799914078e-11</v>
       </c>
     </row>
     <row r="58">
@@ -3639,10 +3639,10 @@
         </is>
       </c>
       <c r="N58" t="n">
-        <v>1.978629999999997</v>
+        <v>1</v>
       </c>
       <c r="O58" t="n">
-        <v>6.153539299999984e-106</v>
+        <v>3.109999999999996e-106</v>
       </c>
     </row>
     <row r="59">
@@ -3694,10 +3694,10 @@
         </is>
       </c>
       <c r="N59" t="n">
-        <v>1.658680000000004</v>
+        <v>1</v>
       </c>
       <c r="O59" t="n">
-        <v>5.058974037942318e-08</v>
+        <v>3.050000022875e-08</v>
       </c>
     </row>
     <row r="60">
@@ -3749,10 +3749,10 @@
         </is>
       </c>
       <c r="N60" t="n">
-        <v>2.392270000000001</v>
+        <v>1.392270000000001</v>
       </c>
       <c r="O60" t="n">
-        <v>6.172056603579795e-09</v>
+        <v>3.592056602083394e-09</v>
       </c>
     </row>
   </sheetData>

</xml_diff>